<commit_message>
Update to the final report
</commit_message>
<xml_diff>
--- a/writeup/figures/Human Accuracies.xlsx
+++ b/writeup/figures/Human Accuracies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evan_\OneDrive\Documents\GitHub\bike-friendly-street-classifier\writeup\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1DFDAE-0BF1-465B-94C6-0842C1904421}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8788125-BB36-4033-B425-CD16D356986E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="5835" xr2:uid="{7BEC9C35-FF31-4740-A565-87F69C7AF99E}"/>
   </bookViews>
@@ -28,6 +28,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Average samples done per user</t>
+  </si>
+  <si>
+    <t>Cumulative Mean</t>
+  </si>
+  <si>
+    <t>Per Person std deviation</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4B308D-6CCC-4788-A452-C99DCFCE0098}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1">
         <v>105</v>
       </c>
@@ -419,7 +433,7 @@
         <v>63.99999999999995</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>222</v>
       </c>
@@ -431,7 +445,7 @@
         <v>139.99999999999986</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>75</v>
       </c>
@@ -442,8 +456,11 @@
         <f t="shared" si="0"/>
         <v>49.99999999999995</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>6</v>
       </c>
@@ -454,8 +471,12 @@
         <f t="shared" si="0"/>
         <v>1.9999999999999978</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G4">
+        <f>AVERAGE(A1:A17)</f>
+        <v>77.235294117647058</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -467,7 +488,7 @@
         <v>45.999999999999922</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>38</v>
       </c>
@@ -478,8 +499,11 @@
         <f t="shared" si="0"/>
         <v>27.999999999999964</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -490,8 +514,12 @@
         <f t="shared" si="0"/>
         <v>1.9999999999999949</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G7">
+        <f>D22</f>
+        <v>0.59481987776085254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>201</v>
       </c>
@@ -503,7 +531,7 @@
         <v>118.99999999999982</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>100</v>
       </c>
@@ -514,8 +542,11 @@
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>101</v>
       </c>
@@ -526,8 +557,12 @@
         <f t="shared" si="0"/>
         <v>67.999999999999972</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G10">
+        <f>_xlfn.STDEV.P(B1:B17)</f>
+        <v>0.12231398502045826</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -539,7 +574,7 @@
         <v>4.9995000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>27</v>
       </c>
@@ -551,7 +586,7 @@
         <v>10.999999999999989</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>51</v>
       </c>
@@ -563,7 +598,7 @@
         <v>27.999000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>50</v>
       </c>
@@ -575,7 +610,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>101</v>
       </c>
@@ -587,7 +622,7 @@
         <v>49.999999499999994</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>18</v>
       </c>

</xml_diff>